<commit_message>
Update GreenSite_4_12_24_Antiviral replication Jessica Smith.xlsx
</commit_message>
<xml_diff>
--- a/Virtual screen GS raw data/GreenSite_4_12_24_Antiviral replication Jessica Smith.xlsx
+++ b/Virtual screen GS raw data/GreenSite_4_12_24_Antiviral replication Jessica Smith.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smijessi/Documents/jessicasmith/Data/AVIDD/RdRp/Green site/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uccaris_ucl_ac_uk/Documents/GitHub/CNP18-DENVRdrp-VirtualScreen/Virtual screen GS raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C759FE1-12E8-5045-9004-F406A4A79709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3C759FE1-12E8-5045-9004-F406A4A79709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AF7144B-98C2-4776-B329-F29B012A8EBD}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="37140" windowHeight="19700" xr2:uid="{10828EC6-2BD3-FB48-BAEA-8C9EE13D215D}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{10828EC6-2BD3-FB48-BAEA-8C9EE13D215D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,17 +485,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD3FEE-2696-D446-9DEB-AB420385AE09}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="8" width="18.6640625" customWidth="1"/>
+    <col min="2" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -519,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -571,7 +573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -597,7 +599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -623,7 +625,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>